<commit_message>
wcvp authority omission fixed
</commit_message>
<xml_diff>
--- a/splists_out/wright_nomenclature_R_20210224_WCVP_CHANGES_2026-02-26.xlsx
+++ b/splists_out/wright_nomenclature_R_20210224_WCVP_CHANGES_2026-02-26.xlsx
@@ -40997,7 +40997,7 @@
       </c>
       <c r="AJ203" t="inlineStr">
         <is>
-          <t>Quisumb.</t>
+          <t>C.DC.</t>
         </is>
       </c>
       <c r="AK203" t="inlineStr">
@@ -48455,7 +48455,7 @@
       </c>
       <c r="AJ240" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Pittier</t>
         </is>
       </c>
       <c r="AK240" t="inlineStr">
@@ -52644,7 +52644,7 @@
       </c>
       <c r="AJ261" t="inlineStr">
         <is>
-          <t>NA</t>
+          <t>Pittier</t>
         </is>
       </c>
       <c r="AK261" t="inlineStr">
@@ -56694,7 +56694,7 @@
       </c>
       <c r="AJ281" t="inlineStr">
         <is>
-          <t>(Baker) Baker</t>
+          <t>(L.) Blume</t>
         </is>
       </c>
       <c r="AK281" t="inlineStr">

</xml_diff>